<commit_message>
Update Collection DSS exports
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_DM.xlsx
+++ b/curation/draft/collection/collection_specialization_DM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94E959A-FA9E-4350-860B-E880E157F905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE142DDB-7172-406F-A1E8-B19F01F98FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Collection_DM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_DM!$A$1:$AG$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_DM!$A$1:$AG$16</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="96">
   <si>
     <t>package_date</t>
   </si>
@@ -287,13 +287,37 @@
   </si>
   <si>
     <t>Specify Other Race</t>
+  </si>
+  <si>
+    <t>Date Only</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>SEX_MF</t>
+  </si>
+  <si>
+    <t>Sex Male Female Only</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>F;M</t>
+  </si>
+  <si>
+    <t>Female;Male</t>
+  </si>
+  <si>
+    <t>BRTHDTC_SHORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +342,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9.5"/>
+      <color rgb="FF0000FF"/>
+      <name val="Albany AMT"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -333,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -371,11 +401,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -411,6 +456,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG14"/>
+  <dimension ref="A1:AG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,57 +1072,74 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>72</v>
+      <c r="H5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="N5" t="s">
-        <v>73</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q5" s="12">
+        <v>85</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="14">
         <v>1</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="14">
+        <v>10</v>
+      </c>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="S5" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5">
-        <v>10</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>81</v>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE5" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
@@ -1094,41 +1161,42 @@
       <c r="H6" t="s">
         <v>34</v>
       </c>
+      <c r="J6" s="2"/>
       <c r="K6" t="s">
         <v>34</v>
       </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="s">
-        <v>34</v>
+      <c r="L6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="Q6" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S6" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="T6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AD6" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="AE6" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>33</v>
       </c>
@@ -1151,57 +1219,42 @@
         <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="N7" t="s">
-        <v>45</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>86</v>
+        <v>42</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="Q7" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R7" t="s">
         <v>43</v>
       </c>
       <c r="S7" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="T7">
-        <v>20</v>
-      </c>
-      <c r="W7" t="s">
-        <v>47</v>
-      </c>
-      <c r="X7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y7" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="AD7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="AE7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -1213,44 +1266,58 @@
         <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>72</v>
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" t="s">
+        <v>44</v>
       </c>
       <c r="N8" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="S8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="T8">
-        <v>10</v>
-      </c>
-      <c r="Y8"/>
+        <v>20</v>
+      </c>
+      <c r="W8" t="s">
+        <v>47</v>
+      </c>
+      <c r="X8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y8" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>63</v>
+      </c>
       <c r="AD8" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="AE8" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>48</v>
       </c>
@@ -1272,58 +1339,44 @@
       <c r="K9" t="s">
         <v>49</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" t="s">
+        <v>73</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" t="s">
+        <v>40</v>
+      </c>
+      <c r="T9">
+        <v>10</v>
+      </c>
+      <c r="Y9"/>
+      <c r="AD9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
-      </c>
-      <c r="M9" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q9" s="12">
-        <v>2</v>
-      </c>
-      <c r="R9" t="s">
-        <v>43</v>
-      </c>
-      <c r="S9" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9">
-        <v>100</v>
-      </c>
-      <c r="W9" t="s">
-        <v>50</v>
-      </c>
-      <c r="X9" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
@@ -1335,116 +1388,144 @@
         <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>72</v>
+        <v>49</v>
+      </c>
+      <c r="L10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" t="s">
+        <v>49</v>
       </c>
       <c r="N10" t="s">
-        <v>73</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>78</v>
+        <v>48</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="Q10" s="12">
+        <v>2</v>
+      </c>
+      <c r="R10" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10">
+        <v>100</v>
+      </c>
+      <c r="W10" t="s">
+        <v>50</v>
+      </c>
+      <c r="X10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q11" s="14">
         <v>1</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11" s="14">
+        <v>100</v>
+      </c>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="S10" t="s">
-        <v>40</v>
-      </c>
-      <c r="T10">
-        <v>10</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" t="s">
-        <v>52</v>
-      </c>
-      <c r="L11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="12">
-        <v>2</v>
-      </c>
-      <c r="R11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T11">
-        <v>100</v>
-      </c>
-      <c r="W11" t="s">
-        <v>53</v>
-      </c>
-      <c r="X11" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA11" t="s">
+      <c r="W11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="X11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z11" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA11" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AD11" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>52</v>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE11" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
@@ -1456,10 +1537,10 @@
         <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>72</v>
@@ -1470,7 +1551,6 @@
       <c r="N12" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="2"/>
       <c r="P12" s="2" t="s">
         <v>78</v>
       </c>
@@ -1493,12 +1573,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -1506,29 +1586,26 @@
       <c r="E13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="G13" t="s">
         <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="N13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="Q13" s="12">
         <v>2</v>
@@ -1543,28 +1620,28 @@
         <v>100</v>
       </c>
       <c r="W13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="X13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="AA13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="AE13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>56</v>
       </c>
@@ -1577,9 +1654,6 @@
       <c r="E14" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="G14" t="s">
         <v>37</v>
       </c>
@@ -1589,41 +1663,169 @@
       <c r="K14" t="s">
         <v>57</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" t="s">
+        <v>73</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q14" s="12">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" t="s">
+        <v>40</v>
+      </c>
+      <c r="T14">
+        <v>10</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="135" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15" s="12">
+        <v>2</v>
+      </c>
+      <c r="R15" t="s">
+        <v>43</v>
+      </c>
+      <c r="S15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15">
+        <v>100</v>
+      </c>
+      <c r="W15" t="s">
+        <v>59</v>
+      </c>
+      <c r="X15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" t="s">
         <v>62</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M16" t="s">
         <v>62</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q16" s="12">
         <v>3</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R16" t="s">
         <v>43</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S16" t="s">
         <v>46</v>
       </c>
-      <c r="T14">
+      <c r="T16">
         <v>200</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AD16" t="s">
         <v>62</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AG16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://evsexplore.semantics.cancer.gov/evsexplore/concept/ncit/C83217" xr:uid="{139FC7E2-5129-A54A-8064-0A3EC9B6468E}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://evsexplore.semantics.cancer.gov/evsexplore/concept/ncit/C83217" xr:uid="{7EE5EACC-2268-A941-AD1C-9536F3A5845B}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://evsexplore.semantics.cancer.gov/evsexplore/concept/ncit/C83217" xr:uid="{763BC429-BC4A-5644-A069-B0FBFA4F3225}"/>
+    <hyperlink ref="N5" r:id="rId1" xr:uid="{B411ED39-AB72-4C32-B2DD-CC503DD7BEAB}"/>
+    <hyperlink ref="N11" r:id="rId2" xr:uid="{0914D680-48BC-415E-8806-2D38E1E30AE9}"/>
+    <hyperlink ref="W11" r:id="rId3" xr:uid="{1EDF5916-EFC2-4278-97FC-3796322A9ADA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
DM, DS, EG updated to include categories
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_DM.xlsx
+++ b/curation/draft/collection/collection_specialization_DM.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE142DDB-7172-406F-A1E8-B19F01F98FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C088BD6C-DD05-A240-A763-0639333E17EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_DM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_DM!$A$1:$AG$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_DM!$A$1:$AH$16</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="97">
   <si>
     <t>package_date</t>
   </si>
@@ -311,13 +311,16 @@
   </si>
   <si>
     <t>BRTHDTC_SHORT</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,36 +767,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG16"/>
+  <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" style="5"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="47.85546875" customWidth="1"/>
-    <col min="16" max="16" width="41.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" style="12" customWidth="1"/>
-    <col min="18" max="18" width="18.7109375" customWidth="1"/>
-    <col min="19" max="22" width="8.85546875" customWidth="1"/>
-    <col min="25" max="25" width="21.7109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="28.7109375" style="2" customWidth="1"/>
-    <col min="27" max="27" width="19" customWidth="1"/>
-    <col min="28" max="28" width="22" customWidth="1"/>
-    <col min="29" max="29" width="15" customWidth="1"/>
-    <col min="31" max="31" width="16" customWidth="1"/>
+    <col min="10" max="11" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="47.83203125" customWidth="1"/>
+    <col min="17" max="17" width="41.1640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="18.5" style="12" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" customWidth="1"/>
+    <col min="20" max="23" width="8.83203125" customWidth="1"/>
+    <col min="26" max="26" width="21.6640625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="28.6640625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="19" customWidth="1"/>
+    <col min="29" max="29" width="22" customWidth="1"/>
+    <col min="30" max="30" width="15" customWidth="1"/>
+    <col min="32" max="32" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,76 +828,79 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="16">
       <c r="A2" s="7"/>
       <c r="B2" t="s">
         <v>71</v>
@@ -917,53 +923,54 @@
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="M2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" t="s">
         <v>73</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="7"/>
+      <c r="Q2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="R2" s="11">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>39</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>40</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>10</v>
       </c>
-      <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
-      <c r="Y2" s="9"/>
+      <c r="Y2" s="7"/>
       <c r="Z2" s="9"/>
-      <c r="AA2" s="7"/>
+      <c r="AA2" s="9"/>
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
-      <c r="AD2" t="s">
-        <v>81</v>
-      </c>
+      <c r="AD2" s="7"/>
       <c r="AE2" t="s">
         <v>81</v>
       </c>
-      <c r="AF2" s="7"/>
+      <c r="AF2" t="s">
+        <v>81</v>
+      </c>
       <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
     </row>
-    <row r="3" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="16">
       <c r="B3" t="s">
         <v>71</v>
       </c>
@@ -983,41 +990,42 @@
         <v>41</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="L3" t="s">
-        <v>38</v>
       </c>
       <c r="M3" t="s">
         <v>38</v>
       </c>
       <c r="N3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>43</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>40</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>10</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>41</v>
       </c>
       <c r="AE3" t="s">
         <v>41</v>
       </c>
+      <c r="AF3" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="16">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -1037,41 +1045,42 @@
         <v>41</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="L4" t="s">
-        <v>83</v>
       </c>
       <c r="M4" t="s">
         <v>83</v>
       </c>
       <c r="N4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" t="s">
         <v>85</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="R4" s="12">
         <v>3</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>39</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>84</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>5</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>41</v>
       </c>
       <c r="AE4" t="s">
         <v>41</v>
       </c>
+      <c r="AF4" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="16">
       <c r="A5" s="14"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -1096,53 +1105,54 @@
       <c r="J5" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="14"/>
+      <c r="L5" s="16" t="s">
         <v>89</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="M5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
         <v>85</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="P5" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="14">
+      <c r="Q5" s="16"/>
+      <c r="R5" s="14">
         <v>1</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="S5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="T5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="14">
+      <c r="U5" s="14">
         <v>10</v>
       </c>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14" t="s">
+      <c r="V5" s="14"/>
+      <c r="W5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="W5" s="14"/>
       <c r="X5" s="14"/>
-      <c r="Y5" s="16"/>
+      <c r="Y5" s="14"/>
       <c r="Z5" s="16"/>
-      <c r="AA5" s="14"/>
+      <c r="AA5" s="16"/>
       <c r="AB5" s="14"/>
       <c r="AC5" s="14"/>
-      <c r="AD5" s="14" t="s">
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AE5" s="16" t="s">
+      <c r="AF5" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="16">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -1162,41 +1172,42 @@
         <v>34</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" t="s">
+      <c r="K6" s="2"/>
+      <c r="L6" t="s">
         <v>34</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="M6" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" t="s">
         <v>73</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="R6" s="12">
         <v>1</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>39</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>40</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>10</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>81</v>
       </c>
       <c r="AE6" t="s">
         <v>81</v>
       </c>
+      <c r="AF6" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="16">
       <c r="B7" t="s">
         <v>33</v>
       </c>
@@ -1215,9 +1226,6 @@
       <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="K7" t="s">
-        <v>34</v>
-      </c>
       <c r="L7" t="s">
         <v>34</v>
       </c>
@@ -1225,31 +1233,34 @@
         <v>34</v>
       </c>
       <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="R7" s="12">
         <v>2</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>43</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>65</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>3</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>34</v>
       </c>
       <c r="AE7" t="s">
         <v>34</v>
       </c>
+      <c r="AF7" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="8" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="32">
       <c r="B8" t="s">
         <v>33</v>
       </c>
@@ -1268,56 +1279,56 @@
       <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>34</v>
-      </c>
-      <c r="L8" t="s">
-        <v>44</v>
       </c>
       <c r="M8" t="s">
         <v>44</v>
       </c>
       <c r="N8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="Q8" s="12">
+      <c r="R8" s="12">
         <v>3</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>43</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>46</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>20</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>47</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>44</v>
       </c>
-      <c r="Y8" s="10" t="s">
+      <c r="Z8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>63</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>44</v>
       </c>
       <c r="AE8" t="s">
         <v>44</v>
       </c>
+      <c r="AF8" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="16">
       <c r="B9" t="s">
         <v>48</v>
       </c>
@@ -1336,42 +1347,42 @@
       <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>49</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="M9" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" t="s">
         <v>73</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q9" s="12">
+      <c r="R9" s="12">
         <v>1</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>39</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>40</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>10</v>
       </c>
-      <c r="Y9"/>
-      <c r="AD9" t="s">
-        <v>81</v>
-      </c>
+      <c r="Z9"/>
       <c r="AE9" t="s">
         <v>81</v>
       </c>
+      <c r="AF9" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="10" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="16">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -1390,9 +1401,6 @@
       <c r="H10" t="s">
         <v>49</v>
       </c>
-      <c r="K10" t="s">
-        <v>49</v>
-      </c>
       <c r="L10" t="s">
         <v>49</v>
       </c>
@@ -1400,46 +1408,49 @@
         <v>49</v>
       </c>
       <c r="N10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q10" s="12">
+      <c r="R10" s="12">
         <v>2</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>43</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>46</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>100</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>50</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>49</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Z10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="AA10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>63</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>49</v>
       </c>
       <c r="AE10" t="s">
         <v>49</v>
       </c>
+      <c r="AF10" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="16">
       <c r="A11" s="14"/>
       <c r="B11" t="s">
         <v>48</v>
@@ -1464,63 +1475,64 @@
       <c r="J11" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K11" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="L11" s="14" t="s">
+      <c r="K11" s="14"/>
+      <c r="L11" s="16" t="s">
         <v>49</v>
       </c>
       <c r="M11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" t="s">
         <v>48</v>
       </c>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16" t="s">
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="R11" s="14">
         <v>1</v>
       </c>
-      <c r="R11" s="14" t="s">
+      <c r="S11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="T11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="T11" s="14">
+      <c r="U11" s="14">
         <v>100</v>
       </c>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14" t="s">
+      <c r="V11" s="14"/>
+      <c r="W11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="W11" s="15" t="s">
+      <c r="X11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="X11" s="14" t="s">
+      <c r="Y11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="Y11" s="16" t="s">
+      <c r="Z11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="Z11" s="16" t="s">
+      <c r="AA11" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="AA11" s="14" t="s">
+      <c r="AB11" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AB11" s="14"/>
       <c r="AC11" s="14"/>
-      <c r="AD11" s="14" t="s">
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AE11" s="16" t="s">
+      <c r="AF11" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="16">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1539,41 +1551,41 @@
       <c r="H12" t="s">
         <v>52</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>52</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="M12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" t="s">
         <v>73</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="R12" s="12">
         <v>1</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>39</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>40</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>10</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>81</v>
       </c>
       <c r="AE12" t="s">
         <v>81</v>
       </c>
+      <c r="AF12" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="13" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="48">
       <c r="B13" t="s">
         <v>51</v>
       </c>
@@ -1592,9 +1604,6 @@
       <c r="H13" t="s">
         <v>52</v>
       </c>
-      <c r="K13" t="s">
-        <v>52</v>
-      </c>
       <c r="L13" t="s">
         <v>52</v>
       </c>
@@ -1602,46 +1611,49 @@
         <v>52</v>
       </c>
       <c r="N13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" t="s">
         <v>51</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="R13" s="12">
         <v>2</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>43</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>46</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>100</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>53</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>52</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Z13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="AA13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AB13" t="s">
         <v>63</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>52</v>
       </c>
       <c r="AE13" t="s">
         <v>52</v>
       </c>
+      <c r="AF13" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="16">
       <c r="B14" t="s">
         <v>56</v>
       </c>
@@ -1660,42 +1672,42 @@
       <c r="H14" t="s">
         <v>57</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>57</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="M14" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O14" t="s">
         <v>73</v>
       </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2" t="s">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="R14" s="12">
         <v>1</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>39</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>40</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>10</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>81</v>
       </c>
       <c r="AE14" t="s">
         <v>81</v>
       </c>
+      <c r="AF14" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="15" spans="1:33" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="144">
       <c r="B15" t="s">
         <v>56</v>
       </c>
@@ -1717,9 +1729,6 @@
       <c r="H15" t="s">
         <v>57</v>
       </c>
-      <c r="K15" t="s">
-        <v>57</v>
-      </c>
       <c r="L15" t="s">
         <v>57</v>
       </c>
@@ -1727,46 +1736,49 @@
         <v>57</v>
       </c>
       <c r="N15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O15" t="s">
         <v>56</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Q15" s="12">
+      <c r="R15" s="12">
         <v>2</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>43</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>46</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>100</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>59</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>57</v>
       </c>
-      <c r="Y15" s="2" t="s">
+      <c r="Z15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Z15" s="2" t="s">
+      <c r="AA15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>64</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>57</v>
       </c>
       <c r="AE15" t="s">
         <v>57</v>
       </c>
+      <c r="AF15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="16" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="32">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1788,44 +1800,44 @@
       <c r="H16" t="s">
         <v>57</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>57</v>
-      </c>
-      <c r="L16" t="s">
-        <v>62</v>
       </c>
       <c r="M16" t="s">
         <v>62</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="N16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="R16" s="12">
         <v>3</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>43</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>46</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>200</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>62</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AF16" s="2" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AH16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N5" r:id="rId1" xr:uid="{B411ED39-AB72-4C32-B2DD-CC503DD7BEAB}"/>
-    <hyperlink ref="N11" r:id="rId2" xr:uid="{0914D680-48BC-415E-8806-2D38E1E30AE9}"/>
-    <hyperlink ref="W11" r:id="rId3" xr:uid="{1EDF5916-EFC2-4278-97FC-3796322A9ADA}"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{B411ED39-AB72-4C32-B2DD-CC503DD7BEAB}"/>
+    <hyperlink ref="O11" r:id="rId2" xr:uid="{0914D680-48BC-415E-8806-2D38E1E30AE9}"/>
+    <hyperlink ref="X11" r:id="rId3" xr:uid="{1EDF5916-EFC2-4278-97FC-3796322A9ADA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added derivation columns (blank - AGE has only the collected age, not the derived age)
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_DM.xlsx
+++ b/curation/draft/collection/collection_specialization_DM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C088BD6C-DD05-A240-A763-0639333E17EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0BC9DB-B4BE-6C4A-AEC7-6908CF488BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Collection_DM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_DM!$A$1:$AH$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_DM!$A$1:$AJ$16</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="99">
   <si>
     <t>package_date</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -767,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH16"/>
+  <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -787,16 +793,16 @@
     <col min="17" max="17" width="41.1640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="18.5" style="12" customWidth="1"/>
     <col min="19" max="19" width="18.6640625" customWidth="1"/>
-    <col min="20" max="23" width="8.83203125" customWidth="1"/>
-    <col min="26" max="26" width="21.6640625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="28.6640625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="19" customWidth="1"/>
-    <col min="29" max="29" width="22" customWidth="1"/>
-    <col min="30" max="30" width="15" customWidth="1"/>
-    <col min="32" max="32" width="16" customWidth="1"/>
+    <col min="20" max="25" width="8.83203125" customWidth="1"/>
+    <col min="28" max="28" width="21.6640625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="28.6640625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="19" customWidth="1"/>
+    <col min="31" max="31" width="22" customWidth="1"/>
+    <col min="32" max="32" width="15" customWidth="1"/>
+    <col min="34" max="34" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16">
+    <row r="1" spans="1:36" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,40 +873,46 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="16">
+    <row r="2" spans="1:36" ht="16">
       <c r="A2" s="7"/>
       <c r="B2" t="s">
         <v>71</v>
@@ -956,21 +968,23 @@
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
       <c r="AD2" s="7"/>
-      <c r="AE2" t="s">
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" t="s">
         <v>81</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>81</v>
       </c>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
     </row>
-    <row r="3" spans="1:34" ht="16">
+    <row r="3" spans="1:36" ht="16">
       <c r="B3" t="s">
         <v>71</v>
       </c>
@@ -1018,14 +1032,14 @@
       <c r="U3">
         <v>10</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="16">
+    <row r="4" spans="1:36" ht="16">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -1073,14 +1087,14 @@
       <c r="U4">
         <v>5</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>41</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="16">
+    <row r="5" spans="1:36" ht="16">
       <c r="A5" s="14"/>
       <c r="B5" t="s">
         <v>71</v>
@@ -1140,19 +1154,21 @@
       </c>
       <c r="X5" s="14"/>
       <c r="Y5" s="14"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
       <c r="AD5" s="14"/>
-      <c r="AE5" s="14" t="s">
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AF5" s="16" t="s">
+      <c r="AH5" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="16">
+    <row r="6" spans="1:36" ht="16">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -1200,14 +1216,14 @@
       <c r="U6">
         <v>10</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>81</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="16">
+    <row r="7" spans="1:36" ht="16">
       <c r="B7" t="s">
         <v>33</v>
       </c>
@@ -1253,14 +1269,14 @@
       <c r="U7">
         <v>3</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>34</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="32">
+    <row r="8" spans="1:36" ht="32">
       <c r="B8" t="s">
         <v>33</v>
       </c>
@@ -1306,29 +1322,29 @@
       <c r="U8">
         <v>20</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>47</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA8" t="s">
         <v>44</v>
       </c>
-      <c r="Z8" s="10" t="s">
+      <c r="AB8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AD8" t="s">
         <v>63</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>44</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="16">
+    <row r="9" spans="1:36" ht="16">
       <c r="B9" t="s">
         <v>48</v>
       </c>
@@ -1374,15 +1390,15 @@
       <c r="U9">
         <v>10</v>
       </c>
-      <c r="Z9"/>
-      <c r="AE9" t="s">
+      <c r="AB9"/>
+      <c r="AG9" t="s">
         <v>81</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AH9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="16">
+    <row r="10" spans="1:36" ht="16">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -1428,29 +1444,29 @@
       <c r="U10">
         <v>100</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Z10" t="s">
         <v>50</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AA10" t="s">
         <v>49</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="AB10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AC10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AD10" t="s">
         <v>63</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AG10" t="s">
         <v>49</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="16">
+    <row r="11" spans="1:36" ht="16">
       <c r="A11" s="14"/>
       <c r="B11" t="s">
         <v>48</v>
@@ -1508,31 +1524,33 @@
       <c r="W11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="X11" s="15" t="s">
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="Y11" s="14" t="s">
+      <c r="AA11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="Z11" s="16" t="s">
+      <c r="AB11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="AA11" s="16" t="s">
+      <c r="AC11" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="AB11" s="14" t="s">
+      <c r="AD11" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14" t="s">
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AF11" s="16" t="s">
+      <c r="AH11" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="16">
+    <row r="12" spans="1:36" ht="16">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1578,14 +1596,14 @@
       <c r="U12">
         <v>10</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>81</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AH12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="48">
+    <row r="13" spans="1:36" ht="48">
       <c r="B13" t="s">
         <v>51</v>
       </c>
@@ -1631,29 +1649,29 @@
       <c r="U13">
         <v>100</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Z13" t="s">
         <v>53</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AA13" t="s">
         <v>52</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="AB13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AA13" s="2" t="s">
+      <c r="AC13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AD13" t="s">
         <v>63</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AG13" t="s">
         <v>52</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AH13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="16">
+    <row r="14" spans="1:36" ht="16">
       <c r="B14" t="s">
         <v>56</v>
       </c>
@@ -1700,14 +1718,14 @@
       <c r="U14">
         <v>10</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AG14" t="s">
         <v>81</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AH14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="144">
+    <row r="15" spans="1:36" ht="144">
       <c r="B15" t="s">
         <v>56</v>
       </c>
@@ -1756,29 +1774,29 @@
       <c r="U15">
         <v>100</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Z15" t="s">
         <v>59</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="AA15" t="s">
         <v>57</v>
       </c>
-      <c r="Z15" s="2" t="s">
+      <c r="AB15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AA15" s="2" t="s">
+      <c r="AC15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AD15" t="s">
         <v>64</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AG15" t="s">
         <v>57</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AH15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="32">
+    <row r="16" spans="1:36" ht="32">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1824,20 +1842,20 @@
       <c r="U16">
         <v>200</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AG16" t="s">
         <v>62</v>
       </c>
-      <c r="AF16" s="2" t="s">
+      <c r="AH16" s="2" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="O5" r:id="rId1" xr:uid="{B411ED39-AB72-4C32-B2DD-CC503DD7BEAB}"/>
     <hyperlink ref="O11" r:id="rId2" xr:uid="{0914D680-48BC-415E-8806-2D38E1E30AE9}"/>
-    <hyperlink ref="X11" r:id="rId3" xr:uid="{1EDF5916-EFC2-4278-97FC-3796322A9ADA}"/>
+    <hyperlink ref="Z11" r:id="rId3" xr:uid="{1EDF5916-EFC2-4278-97FC-3796322A9ADA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>